<commit_message>
adding supplementary table 4
</commit_message>
<xml_diff>
--- a/manuscript/Figures_&_tables/Supplementary Table 4 ANOVAs on RYTs.xlsx
+++ b/manuscript/Figures_&_tables/Supplementary Table 4 ANOVAs on RYTs.xlsx
@@ -50,33 +50,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>28581438.5181144</t>
-  </si>
-  <si>
-    <t>522.105734881762</t>
-  </si>
-  <si>
-    <t>1.0254330931424e-38</t>
-  </si>
-  <si>
-    <t>1375468.13007029</t>
-  </si>
-  <si>
-    <t>64.228487439369</t>
-  </si>
-  <si>
-    <t>4.39798437774634e-12</t>
-  </si>
-  <si>
-    <t>19672393.1539865</t>
-  </si>
-  <si>
-    <t>144.486753435827</t>
-  </si>
-  <si>
-    <t>3.03727816568941e-20</t>
-  </si>
-  <si>
     <t>RYT computed on Shoot biomass (mg)</t>
   </si>
   <si>
@@ -84,6 +57,33 @@
   </si>
   <si>
     <t>RYT computed on Total biomass (mg)</t>
+  </si>
+  <si>
+    <t>0.083913</t>
+  </si>
+  <si>
+    <t>26.228</t>
+  </si>
+  <si>
+    <t>4.326e-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.070777</t>
+  </si>
+  <si>
+    <t>32.555</t>
+  </si>
+  <si>
+    <t>5.3e-07</t>
+  </si>
+  <si>
+    <t>0.087204</t>
+  </si>
+  <si>
+    <t>34.873</t>
+  </si>
+  <si>
+    <t>2.56e-07</t>
   </si>
 </sst>
 </file>
@@ -423,18 +423,17 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -445,7 +444,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -473,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -485,15 +484,15 @@
         <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -521,10 +520,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -533,15 +532,15 @@
         <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -569,10 +568,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -581,10 +580,10 @@
         <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>